<commit_message>
se suben mas mediciones
</commit_message>
<xml_diff>
--- a/medicionesCaracteristicaDeSalida.xlsx
+++ b/medicionesCaracteristicaDeSalida.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuel Mollon\Dropbox\ELECTRO 2\electro2-TP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malen\Desktop\ELECTRONICA II\electro2-TP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0062E9C-3C7A-4795-8767-06B16D5FC789}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1DDD92-2B4E-4360-94C7-7B71EC71C7F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A8DB24F2-A3C7-4075-9AAC-49F781B77E81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A8DB24F2-A3C7-4075-9AAC-49F781B77E81}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -101,7 +101,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -332,7 +332,7 @@
             <c:numRef>
               <c:f>Hoja1!$C$2:$C$21</c:f>
               <c:numCache>
-                <c:formatCode>0,00E+00</c:formatCode>
+                <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>3.917748917748918E-5</c:v>
@@ -1188,7 +1188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1484,15 +1484,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA81BF6-8737-4BDC-A8A6-B029AD8877A6}">
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1512,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>231000</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>9.0250000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>160000</v>
       </c>
@@ -1548,7 +1548,7 @@
         <v>9.0210000000000008</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>90000</v>
       </c>
@@ -1566,7 +1566,7 @@
         <v>9.02</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>30000</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>18000</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>15000</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>1.9E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>13000</v>
       </c>
@@ -1650,7 +1650,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>12000</v>
       </c>
@@ -1665,13 +1665,13 @@
         <v>524</v>
       </c>
       <c r="L9">
-        <v>8.99</v>
+        <v>9</v>
       </c>
       <c r="M9">
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>11000</v>
       </c>
@@ -1686,13 +1686,13 @@
         <v>360</v>
       </c>
       <c r="L10">
-        <v>8.84</v>
+        <v>9</v>
       </c>
       <c r="M10">
-        <v>3.5999999999999997E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10000</v>
       </c>
@@ -1707,13 +1707,13 @@
         <v>170</v>
       </c>
       <c r="L11">
-        <v>7.08</v>
+        <v>9</v>
       </c>
       <c r="M11">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>8000</v>
       </c>
@@ -1728,13 +1728,13 @@
         <v>130</v>
       </c>
       <c r="L12">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="M12">
-        <v>6.2E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>6000</v>
       </c>
@@ -1746,16 +1746,16 @@
         <v>1.4666666666666667E-3</v>
       </c>
       <c r="K13" s="1">
-        <v>6</v>
+        <v>90</v>
       </c>
       <c r="L13">
-        <v>8.6</v>
+        <v>9</v>
       </c>
       <c r="M13">
-        <v>1.45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.16200000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5000</v>
       </c>
@@ -1767,16 +1767,16 @@
         <v>1.7399999999999998E-3</v>
       </c>
       <c r="K14" s="1">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="L14">
-        <v>6.46</v>
+        <v>9</v>
       </c>
       <c r="M14">
-        <v>1.29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>4000</v>
       </c>
@@ -1788,16 +1788,16 @@
         <v>2.15E-3</v>
       </c>
       <c r="K15" s="1">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="L15">
-        <v>4.67</v>
+        <v>9</v>
       </c>
       <c r="M15">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>3000</v>
       </c>
@@ -1809,16 +1809,16 @@
         <v>2.7666666666666668E-3</v>
       </c>
       <c r="K16" s="1">
-        <v>3</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="L16">
-        <v>3.22</v>
+        <v>8.99</v>
       </c>
       <c r="M16">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>1400</v>
       </c>
@@ -1830,16 +1830,16 @@
         <v>5.5714285714285709E-3</v>
       </c>
       <c r="K17" s="1">
-        <v>2</v>
+        <v>6.7</v>
       </c>
       <c r="L17">
-        <v>2.0169999999999999</v>
+        <v>8.99</v>
       </c>
       <c r="M17">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>800</v>
       </c>
@@ -1851,34 +1851,87 @@
         <v>9.6249999999999999E-3</v>
       </c>
       <c r="K18" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="L18">
-        <v>0.97</v>
+        <v>8.6</v>
       </c>
       <c r="M18">
-        <v>0.92</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
       </c>
       <c r="K19" s="1">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L19">
-        <v>0</v>
+        <v>6.46</v>
       </c>
       <c r="M19">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="e">
         <f t="shared" si="0"/>
         <v>#DIV/0!</v>
+      </c>
+      <c r="K20" s="1">
+        <v>4</v>
+      </c>
+      <c r="L20">
+        <v>4.67</v>
+      </c>
+      <c r="M20">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="1">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>3.22</v>
+      </c>
+      <c r="M21">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K22" s="1">
+        <v>2</v>
+      </c>
+      <c r="L22">
+        <v>2.0169999999999999</v>
+      </c>
+      <c r="M22">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K23" s="1">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>0.97</v>
+      </c>
+      <c r="M23">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K24" s="1">
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0.87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>